<commit_message>
Fix controlled vocabularies documentation
</commit_message>
<xml_diff>
--- a/data-requirements/data-requirements.xlsx
+++ b/data-requirements/data-requirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\tandcatap\data-requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\tandcatap\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0A2800-8EC0-44C2-A931-A953D68C43BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EEC722-434C-4825-853C-45C46CBA8649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>dct:title</t>
   </si>
@@ -67,9 +67,6 @@
     <t>TANGENT Data Requirements</t>
   </si>
   <si>
-    <t>Data Requirements for data sources enabling the TANGENT solution.</t>
-  </si>
-  <si>
     <t>Road Transport Network</t>
   </si>
   <si>
@@ -137,6 +134,45 @@
   </si>
   <si>
     <t>DRT Fleet Characteristics</t>
+  </si>
+  <si>
+    <t>dct:creator</t>
+  </si>
+  <si>
+    <t>Mario Scrocca (Cefriel)</t>
+  </si>
+  <si>
+    <t>dct:publisher</t>
+  </si>
+  <si>
+    <t>TANGENT WP2</t>
+  </si>
+  <si>
+    <t>owl:versionInfo</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>owl:versionIRI</t>
+  </si>
+  <si>
+    <t>owl:priorVersion</t>
+  </si>
+  <si>
+    <t>dct:license</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
+    <t>http://purl.org/ontology/bibo/status</t>
+  </si>
+  <si>
+    <t>Published Controlled Vocabulary</t>
+  </si>
+  <si>
+    <t>Controlled vocabulary for the list of data requirements defined in TANGENT.</t>
   </si>
 </sst>
 </file>
@@ -201,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -217,6 +253,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,7 +563,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -534,23 +571,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="89.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="89.44140625" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -558,7 +595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -567,245 +604,307 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="str">
+        <f>_xlfn.CONCAT(B1,"/",B6)</f>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/1.0.0</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>_xlfn.CONCAT("https://knowledge.c-innovationhub.com/tangent/data-requirements/",SUBSTITUTE(LOWER(B15)," ","-"))</f>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-transport-network</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f>_xlfn.CONCAT("https://knowledge.c-innovationhub.com/tangent/data-requirements/",SUBSTITUTE(LOWER(B8)," ","-"))</f>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-transport-network</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f t="shared" ref="A16:A37" si="0">_xlfn.CONCAT("https://knowledge.c-innovationhub.com/tangent/data-requirements/",SUBSTITUTE(LOWER(B16)," ","-"))</f>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-equipment-position</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f t="shared" ref="A9:A30" si="0">_xlfn.CONCAT("https://knowledge.c-innovationhub.com/tangent/data-requirements/",SUBSTITUTE(LOWER(B9)," ","-"))</f>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-equipment-position</v>
-      </c>
-      <c r="B9" s="5" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-network</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-network</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-transport-network-events</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-transport-network-events</v>
-      </c>
-      <c r="B11" s="5" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-network-events</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-network-events</v>
-      </c>
-      <c r="B12" s="5" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-transport-network-incidents</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-transport-network-incidents</v>
-      </c>
-      <c r="B13" s="5" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-network-incidents</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-network-incidents</v>
-      </c>
-      <c r="B14" s="5" t="s">
+    <row r="22" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-traffic-measurements</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-traffic-measurements</v>
-      </c>
-      <c r="B15" s="5" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/floating-vehicle-data</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/floating-vehicle-data</v>
-      </c>
-      <c r="B16" s="5" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-travel-times</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/road-travel-times</v>
-      </c>
-      <c r="B17" s="5" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-schedules-and-lines</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-schedules-and-lines</v>
-      </c>
-      <c r="B18" s="5" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-ticket-validation-data</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-ticket-validation-data</v>
-      </c>
-      <c r="B19" s="5" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/floating-public-transport-vehicle-data</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/floating-public-transport-vehicle-data</v>
-      </c>
-      <c r="B20" s="5" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-delays</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-delays</v>
-      </c>
-      <c r="B21" s="5" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-occupancy</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/public-transport-occupancy</v>
-      </c>
-      <c r="B22" s="5" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/weather-data</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/weather-data</v>
-      </c>
-      <c r="B23" s="5" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/weather-events</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/weather-events</v>
-      </c>
-      <c r="B24" s="5" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/forecasted-weather-data</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/forecasted-weather-data</v>
-      </c>
-      <c r="B25" s="5" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/holiday-calendar</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/holiday-calendar</v>
-      </c>
-      <c r="B26" s="5" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/influencing-planned-events</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/influencing-planned-events</v>
-      </c>
-      <c r="B27" s="5" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/dcp-policy-zone</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/drt-fleet-characteristics</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f t="shared" si="0"/>
+        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/data-about-other-transportation-modes</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/dcp-policy-zone</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/drt-fleet-characteristics</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <f t="shared" si="0"/>
-        <v>https://knowledge.c-innovationhub.com/tangent/data-requirements/data-about-other-transportation-modes</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{8D37ED2A-6F4C-4B2C-B212-84B5255111B4}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{8D4B0B2E-E1BA-44A6-BA31-55DDA5E60404}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{BCDF7F83-1C89-4966-A89D-079AB6D031C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -815,7 +914,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>